<commit_message>
Added reset/program jumper to board
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanso\Desktop\Projects\Go-Kart 2020\Motor Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Downloads\Motor-Controller-main\Motor-Controller-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF1BD1F-CA76-4084-8D9A-2C4BEE4C4AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B316F97-568D-4E0B-8C82-64B9D7B0AEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2100" yWindow="4635" windowWidth="4425" windowHeight="1020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$F$1:$F$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$F$1:$F$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
   <si>
     <t>Part Number</t>
   </si>
@@ -284,6 +284,30 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/yageo/CC1812KKX7R0BB334/5884830</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>JP3 Conn</t>
+  </si>
+  <si>
+    <t>SAM8980-ND</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount 2 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/TSM-102-01-T-SV/2685536</t>
+  </si>
+  <si>
+    <t>ED3082-ND</t>
+  </si>
+  <si>
+    <t>2 (1 x 2) Position Shunt Connector Black Closed Top 0.100" (2.54mm) Gold</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc/EDJ1G0/2752411</t>
   </si>
 </sst>
 </file>
@@ -887,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K16" sqref="J16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +975,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="19">
-        <f t="shared" ref="G2:G19" si="0">D2*E2</f>
+        <f t="shared" ref="G2:G21" si="0">D2*E2</f>
         <v>4.3600000000000003</v>
       </c>
       <c r="H2" s="8" t="s">
@@ -1338,131 +1362,173 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="23" t="s">
+        <v>82</v>
+      </c>
       <c r="B17" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0.34</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="19">
+        <f>D17*E17</f>
+        <v>0.34</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="19">
+        <f>D18*E18</f>
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D19" s="13">
         <v>0</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E19" s="24">
         <v>0.26</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="19">
+      <c r="F19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+    <row r="20" spans="1:8" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B20" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D20" s="13">
         <v>4</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E20" s="24">
         <v>0.41</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="19">
+      <c r="F20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="19">
         <f t="shared" si="0"/>
         <v>1.64</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H20" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
+    <row r="21" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B21" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D21" s="27">
         <v>1</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E21" s="28">
         <v>0.97</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="19">
+      <c r="F21" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="19">
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H21" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="6" t="s">
+    <row r="22" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="7">
-        <f>SUM(G2:G19)</f>
-        <v>53.28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
+      <c r="G22" s="7">
+        <f>SUM(G2:G21)</f>
+        <v>53.720000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
         <v>22</v>
       </c>
-      <c r="G23">
-        <f>SUMIF(F2:F19,"Mouser",G2:G19)</f>
+      <c r="G25">
+        <f>SUMIF(F2:F21,"Mouser",G2:G21)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24">
-        <f>SUMIF(F2:F19,"Digikey",G2:G19)</f>
-        <v>53.28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26">
+        <f>SUMIF(F2:F21,"Digikey",G2:G21)</f>
+        <v>53.720000000000006</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
@@ -1474,7 +1540,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
@@ -1496,19 +1562,31 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="F1:F20" xr:uid="{6E1E27F3-E074-4B73-9092-3525721CDF08}"/>
+  <autoFilter ref="F1:F22" xr:uid="{6E1E27F3-E074-4B73-9092-3525721CDF08}"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{EC06BA25-5BBF-4256-803F-A9FDB457E9B1}"/>
-    <hyperlink ref="H17" r:id="rId2" xr:uid="{AC81996F-D568-4668-86FA-D435AC539FA0}"/>
+    <hyperlink ref="H19" r:id="rId2" xr:uid="{AC81996F-D568-4668-86FA-D435AC539FA0}"/>
     <hyperlink ref="H15" r:id="rId3" xr:uid="{824F3F0F-8998-4AED-93DD-622B79B65A28}"/>
     <hyperlink ref="H8" r:id="rId4" xr:uid="{FEA59C81-A7B8-4225-9F47-3AFC30030BA9}"/>
     <hyperlink ref="H12" r:id="rId5" xr:uid="{C7647B1F-5AC7-476C-92B6-E61230E0D1CD}"/>
     <hyperlink ref="H13" r:id="rId6" xr:uid="{6D4EA0A2-CFDF-4E3D-9F0E-96E89FBB0A78}"/>
     <hyperlink ref="H14" r:id="rId7" xr:uid="{915E4EB1-02CF-4478-8AAD-416A6829D2AF}"/>
-    <hyperlink ref="H18" r:id="rId8" xr:uid="{BFC3512A-DC63-45F2-9FF7-B4E26C9381EA}"/>
+    <hyperlink ref="H20" r:id="rId8" xr:uid="{BFC3512A-DC63-45F2-9FF7-B4E26C9381EA}"/>
     <hyperlink ref="H9" r:id="rId9" xr:uid="{EC517467-96DF-4B7B-AA7B-7290FF844D5E}"/>
-    <hyperlink ref="H19" r:id="rId10" xr:uid="{A8BA41E3-0DB9-477E-9511-169BFBF38909}"/>
+    <hyperlink ref="H21" r:id="rId10" xr:uid="{A8BA41E3-0DB9-477E-9511-169BFBF38909}"/>
     <hyperlink ref="H16" r:id="rId11" xr:uid="{9B76D1D7-DAF2-447F-AF48-0C187821D5C5}"/>
     <hyperlink ref="H10" r:id="rId12" xr:uid="{DB0DBE1B-D9FA-4F4D-B563-579455B73DCF}"/>
     <hyperlink ref="H11" r:id="rId13" xr:uid="{B98F2375-85D1-43B3-B952-25B29C8270AC}"/>
@@ -1517,6 +1595,8 @@
     <hyperlink ref="H3" r:id="rId16" xr:uid="{2BE8EB22-9255-4BDC-ACF3-9DC6D095A159}"/>
     <hyperlink ref="H6" r:id="rId17" xr:uid="{BC4186EC-63DB-4284-A0BA-CD20D91CD4DD}"/>
     <hyperlink ref="H5" r:id="rId18" xr:uid="{01093E0E-B6AD-4853-BF8A-A79C74181CCD}"/>
+    <hyperlink ref="H17" r:id="rId19" xr:uid="{95D555C0-EBE1-4380-80A7-9D30E3C53F09}"/>
+    <hyperlink ref="H18" r:id="rId20" xr:uid="{633A3627-CEB0-4BEA-AA3F-B5E95C17480B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added mounting holes instead of trying to slide the board into the housing
The 3D printed slide mechanism didn't work because the printer couldn't reproduce the sharp corners
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Downloads\Motor-Controller-main\Motor-Controller-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanso\Desktop\Motor-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B316F97-568D-4E0B-8C82-64B9D7B0AEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B09BA-DC25-4DC3-9DA1-DC21545CC5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -292,15 +292,6 @@
     <t>JP3 Conn</t>
   </si>
   <si>
-    <t>SAM8980-ND</t>
-  </si>
-  <si>
-    <t>Connector Header Surface Mount 2 position 0.100" (2.54mm)</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/samtec-inc/TSM-102-01-T-SV/2685536</t>
-  </si>
-  <si>
     <t>ED3082-ND</t>
   </si>
   <si>
@@ -308,6 +299,15 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc/EDJ1G0/2752411</t>
+  </si>
+  <si>
+    <t>10129379-902004BLF-ND</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole, Right Angle 2 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-icc-fci/10129379-902004BLF/7915980</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K16" sqref="J16:K16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1264,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="19">
         <v>0.28999999999999998</v>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="G13" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>45</v>
@@ -1291,7 +1291,7 @@
         <v>47</v>
       </c>
       <c r="D14" s="12">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E14" s="19">
         <v>0.39</v>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="G14" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5100000000000002</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>48</v>
@@ -1366,26 +1366,26 @@
         <v>82</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D17" s="13">
         <v>1</v>
       </c>
       <c r="E17" s="24">
-        <v>0.34</v>
+        <v>0.1</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="19">
         <f>D17*E17</f>
-        <v>0.34</v>
+        <v>0.1</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
@@ -1393,10 +1393,10 @@
         <v>83</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D18" s="13">
         <v>1</v>
@@ -1412,7 +1412,7 @@
         <v>0.1</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E19" s="24">
         <v>0.26</v>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="G19" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.04</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>29</v>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="G22" s="7">
         <f>SUM(G2:G21)</f>
-        <v>53.720000000000006</v>
+        <v>58.32</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G26">
         <f>SUMIF(F2:F21,"Digikey",G2:G21)</f>
-        <v>53.720000000000006</v>
+        <v>58.32</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1595,8 +1595,8 @@
     <hyperlink ref="H3" r:id="rId16" xr:uid="{2BE8EB22-9255-4BDC-ACF3-9DC6D095A159}"/>
     <hyperlink ref="H6" r:id="rId17" xr:uid="{BC4186EC-63DB-4284-A0BA-CD20D91CD4DD}"/>
     <hyperlink ref="H5" r:id="rId18" xr:uid="{01093E0E-B6AD-4853-BF8A-A79C74181CCD}"/>
-    <hyperlink ref="H17" r:id="rId19" xr:uid="{95D555C0-EBE1-4380-80A7-9D30E3C53F09}"/>
-    <hyperlink ref="H18" r:id="rId20" xr:uid="{633A3627-CEB0-4BEA-AA3F-B5E95C17480B}"/>
+    <hyperlink ref="H18" r:id="rId19" xr:uid="{633A3627-CEB0-4BEA-AA3F-B5E95C17480B}"/>
+    <hyperlink ref="H17" r:id="rId20" xr:uid="{D385A36A-D9FF-4658-A354-7779D952A502}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>